<commit_message>
lanes are added to the spreadsheet, soon the cost will be calculated
</commit_message>
<xml_diff>
--- a/materials.xlsx
+++ b/materials.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="148">
+  <si>
+    <t xml:space="preserve">Вид продукт</t>
+  </si>
   <si>
     <t xml:space="preserve">Примерен продукт</t>
   </si>
@@ -34,102 +37,446 @@
     <t xml:space="preserve">Цена за 1 m алея</t>
   </si>
   <si>
+    <t xml:space="preserve">Маршрут</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Участък</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дължина</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Материали</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Бележки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Минимална цена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Максимална цена</t>
+  </si>
+  <si>
     <t xml:space="preserve">боя - светлозелена или червена</t>
   </si>
   <si>
+    <t xml:space="preserve">Главен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">пл. Марсел Де Бископ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">боя, маркировка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">три “зебри" ~10 m, широки 2 m</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1 L евтина боя; разход 300 ml)</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Васил Левски</t>
+  </si>
+  <si>
+    <t xml:space="preserve">павета или асфалт*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*участъците ще бъдат благоустроени независимо от този проект, не е ясно дали са предвидени велоалеи като на ул. Дунав и ул. Аврам Гачев</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1 L скъпа боя; разход 300 ml)</t>
   </si>
   <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1 L евтина боя; разход 500 ml)</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Щастие</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1 L скъпа боя; разход 500 ml)</t>
   </si>
   <si>
     <t xml:space="preserve">колчета/ограничители</t>
   </si>
   <si>
+    <t xml:space="preserve">Падалски мост</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ограничители</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 m от двете страни</t>
+  </si>
+  <si>
     <t xml:space="preserve">adamarm.com колче 70 cm 1.4 mm</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Дунав</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ограничители и паваж</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85 m участък от готовата велоалея е необяснимо недовършен</t>
+  </si>
+  <si>
     <t xml:space="preserve">adamarm.com огр. Гума 48 cm</t>
   </si>
   <si>
     <t xml:space="preserve">bauhaus.bg огр. пластмаса 20 cm</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Аврам Гачев</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">възможност за разширение</t>
+  </si>
+  <si>
     <t xml:space="preserve">euromatica.bg метално колче</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Юрий Венелин</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ограничители, боя, маркировка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">една "зебра”</t>
+  </si>
+  <si>
     <t xml:space="preserve">adamarm.com колче 70 cm 2 mm</t>
   </si>
   <si>
     <t xml:space="preserve">bariera.eu колче бетониране</t>
   </si>
   <si>
+    <t xml:space="preserve">(ул. Юрий Венелин, край реката)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ограничители, асфалт</t>
+  </si>
+  <si>
     <t xml:space="preserve">bariera.eu стопер 70 cm</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Райчо Каролев</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ограничители, боя, маркириовка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 m от двете страни на пътя</t>
+  </si>
+  <si>
     <t xml:space="preserve">павета – бетон</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Неофит Рилски</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ограничители, маркировка</t>
+  </si>
+  <si>
     <t xml:space="preserve">tashev-galving.com 24x12 cm *претенция</t>
   </si>
   <si>
+    <t xml:space="preserve">асфалт или павета</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дърветата ще бъдат запазени</t>
+  </si>
+  <si>
     <t xml:space="preserve">(паве за 30 лв./m^2)</t>
   </si>
   <si>
     <t xml:space="preserve">tashev-galving.com 20x20 cm</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Капитан Дядо Никола</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ограничители, маркировка, боя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">две "зебри”</t>
+  </si>
+  <si>
     <t xml:space="preserve">tashev-galving.com 10x10 cm</t>
   </si>
   <si>
+    <t xml:space="preserve">ОБЩО:</t>
+  </si>
+  <si>
     <t xml:space="preserve">bauhaus.bg 20x20 cm</t>
   </si>
   <si>
+    <t xml:space="preserve">Централен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(пл. Възраждане)</t>
+  </si>
+  <si>
     <t xml:space="preserve">bauhaus.bg 20x10 cm</t>
   </si>
   <si>
     <t xml:space="preserve">tashev-galving.com 20x10 cm</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Съзаклятие</t>
+  </si>
+  <si>
     <t xml:space="preserve">(паве за 36 лв./m^2)</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Чардафон</t>
+  </si>
+  <si>
+    <t xml:space="preserve">павета</t>
+  </si>
+  <si>
     <t xml:space="preserve">tashev-galving.com 24x12 cm *реални</t>
   </si>
   <si>
     <t xml:space="preserve">подготовка преди павиране</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Баждар</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“зебра”</t>
+  </si>
+  <si>
     <t xml:space="preserve">(100 лв./m^2)</t>
   </si>
   <si>
+    <t xml:space="preserve">мост Игото</t>
+  </si>
+  <si>
+    <t xml:space="preserve">вероятност да отпадне от плана</t>
+  </si>
+  <si>
     <t xml:space="preserve">(250 лв./m^2)</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Софроний Врачански</t>
+  </si>
+  <si>
     <t xml:space="preserve">строене на пътища и асфалтиране</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. 1-ви Май</t>
+  </si>
+  <si>
     <t xml:space="preserve">superkartachi.com (без подготовка)</t>
   </si>
   <si>
+    <t xml:space="preserve">ул. Радион Умников</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Опълченска</t>
+  </si>
+  <si>
+    <t xml:space="preserve">маркировка</t>
+  </si>
+  <si>
     <t xml:space="preserve">*daibau.bg (с подготовка)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Никола Палаузов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Пенчо Славейков</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Априловска</t>
+  </si>
+  <si>
+    <t xml:space="preserve">три "зебри”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Североизточен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Генерал Николов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Георги Кирков</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(тунел под ЖП релси)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">асфалт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">запълване на дупки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Александър Стамболийски</t>
+  </si>
+  <si>
+    <t xml:space="preserve">павета, маркировка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">пл. Белорусия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">шест “зебри”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">маркировка, ограничители</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(мост над Янтра)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*изграждането на втори мост</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Орловска</t>
+  </si>
+  <si>
+    <t xml:space="preserve">асфалт, ограничители</t>
+  </si>
+  <si>
+    <t xml:space="preserve">очистване на растителност</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(паркинг до блок Камчия)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(междублоково пространство)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">неразвита площ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Южен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шиваров мост</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бул. Хемус</t>
+  </si>
+  <si>
+    <t xml:space="preserve">маркировка, павета</t>
+  </si>
+  <si>
+    <t xml:space="preserve">разширяване на тротоара</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(между бул. Хемус и бул. 3-ти март)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бул. 3-ти март</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(до парк Маркотея)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(до изоставения колодрум)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 "зебра”, колодрума е изоставен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Северозападен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Крали Марко</t>
+  </si>
+  <si>
+    <t xml:space="preserve">една “зебра”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бул. Брянска</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Д-р Никола Василиади</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Стефан Караджа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(до градинката в ж.к. Петър Падалски)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">допълнителни опорни стени</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Акация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">боя, маркировка или павета</t>
+  </si>
+  <si>
+    <t xml:space="preserve">може да се изгради пред блока</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Тиха</t>
+  </si>
+  <si>
+    <t xml:space="preserve">боя, маркировка, асфалт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">преасфалтиране, очертаване на паркоместа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бул. Могильов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">двулентова улица с лента за ляв завой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(до блок Катюша)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">изграждане на рампа успоредно на стълбите</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Свищовска</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Лазурна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Парк</t>
+  </si>
+  <si>
+    <t xml:space="preserve">маркировка, боя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">две “зебри”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Алеко Константинов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">преасфалтиране на пътеката близо до алеята</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ул. Д-р Илиев-Детския</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$лв.-402];\-#,##0.00\ [$лв.-402]"/>
-    <numFmt numFmtId="166" formatCode="&quot;широчина &quot;#,###.00&quot; m&quot;"/>
-    <numFmt numFmtId="167" formatCode="&quot;през &quot;#,###.00&quot; m&quot;"/>
+    <numFmt numFmtId="166" formatCode="0&quot; m&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ [$лв.-402];[RED]\-#,##0.00\ [$лв.-402]"/>
+    <numFmt numFmtId="168" formatCode="&quot;широчина &quot;#,###.00&quot; m&quot;"/>
+    <numFmt numFmtId="169" formatCode="&quot;през &quot;#,###.00&quot; m&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -177,7 +524,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,7 +546,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD7D7"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFF6F9D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD4EA6B"/>
+        <bgColor rgb="FFE8F2A1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2A1"/>
+        <bgColor rgb="FFF6F9D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F9D4"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -244,7 +609,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,6 +630,30 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,6 +666,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -285,15 +678,47 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,7 +751,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFF6F9D4"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF6D6D"/>
@@ -342,8 +767,8 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFD4EA6B"/>
+      <rgbColor rgb="FFE8F2A1"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFFA6A6"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -369,7 +794,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -443,6 +868,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -513,6 +939,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -583,6 +1010,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -620,17 +1048,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="25882614"/>
-        <c:axId val="68996129"/>
+        <c:axId val="94550845"/>
+        <c:axId val="79924795"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="25882614"/>
+        <c:axId val="94550845"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -652,7 +1080,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68996129"/>
+        <c:crossAx val="79924795"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -660,7 +1088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68996129"/>
+        <c:axId val="79924795"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -675,7 +1103,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.00\ [$лв.-402];\-#,##0.00\ [$лв.-402]" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00\ [$лв.-402];\-#,##0.00\ [$лв.-402]" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -697,7 +1125,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25882614"/>
+        <c:crossAx val="94550845"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -745,7 +1173,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -819,6 +1247,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -898,6 +1327,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -977,6 +1407,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1023,17 +1454,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="85293107"/>
-        <c:axId val="91293845"/>
+        <c:axId val="68372783"/>
+        <c:axId val="26110669"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85293107"/>
+        <c:axId val="68372783"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1055,7 +1486,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91293845"/>
+        <c:crossAx val="26110669"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1063,7 +1494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91293845"/>
+        <c:axId val="26110669"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1509,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.00\ [$лв.-402];\-#,##0.00\ [$лв.-402]" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00\ [$лв.-402];\-#,##0.00\ [$лв.-402]" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1100,7 +1531,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85293107"/>
+        <c:crossAx val="68372783"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1152,16 +1583,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>26640</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>106560</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>96120</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1169,8 +1600,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11923560" y="218880"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="33275160" y="0"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1182,16 +1613,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>16200</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>806040</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>85680</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>125640</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>61920</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1199,8 +1630,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11903400" y="3475080"/>
-        <a:ext cx="5758920" cy="3234240"/>
+        <a:off x="33241680" y="3657960"/>
+        <a:ext cx="5758560" cy="3233880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1218,58 +1649,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="38.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="19.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="19.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="3" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="38.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="32.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="8" width="45.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="9" width="32.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="I1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10" t="n">
+      <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="10" t="n">
+      <c r="F2" s="17" t="n">
         <v>1.5</v>
       </c>
-      <c r="G2" s="10" t="n">
+      <c r="G2" s="17" t="n">
         <v>2</v>
       </c>
+      <c r="I2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>7.5</v>
@@ -1290,11 +1766,24 @@
         <f aca="false">($D3)*(G$2)</f>
         <v>4.5</v>
       </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="7" t="n">
+        <v>200</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>10</v>
@@ -1315,11 +1804,22 @@
         <f aca="false">($D4)*(G$2)</f>
         <v>6</v>
       </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>7.5</v>
@@ -1340,11 +1840,20 @@
         <f aca="false">($D5)*(G$2)</f>
         <v>7.5</v>
       </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="7" t="n">
+        <v>225</v>
+      </c>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>10</v>
@@ -1365,28 +1874,50 @@
         <f aca="false">($D6)*(G$2)</f>
         <v>10</v>
       </c>
+      <c r="I6" s="18"/>
+      <c r="J6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="7" t="n">
+        <v>95</v>
+      </c>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="11" t="n">
+      <c r="A7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="11" t="n">
+      <c r="F7" s="21" t="n">
         <v>1.5</v>
       </c>
-      <c r="G7" s="11" t="n">
+      <c r="G7" s="21" t="n">
         <v>1</v>
       </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="7" t="n">
+        <v>70</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>15</v>
@@ -1407,11 +1938,24 @@
         <f aca="false">($D8)/(G$7)</f>
         <v>15</v>
       </c>
+      <c r="I8" s="18"/>
+      <c r="J8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="7" t="n">
+        <v>85</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>19</v>
@@ -1432,11 +1976,26 @@
         <f aca="false">($D9)/(G$7)</f>
         <v>19</v>
       </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="7" t="n">
+        <v>195</v>
+      </c>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>19.98</v>
@@ -1457,11 +2016,30 @@
         <f aca="false">($D10)/(G$7)</f>
         <v>19.98</v>
       </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="7" t="n">
+        <v>380</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>25</v>
@@ -1482,11 +2060,24 @@
         <f aca="false">($D11)/(G$7)</f>
         <v>25</v>
       </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="7" t="n">
+        <v>585</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>32</v>
@@ -1507,11 +2098,21 @@
         <f aca="false">($D12)/(G$7)</f>
         <v>32</v>
       </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="7" t="n">
+        <v>125</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>40</v>
@@ -1532,11 +2133,21 @@
         <f aca="false">($D13)/(G$7)</f>
         <v>40</v>
       </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>45</v>
@@ -1557,28 +2168,51 @@
         <f aca="false">($D14)/(G$7)</f>
         <v>45</v>
       </c>
+      <c r="I14" s="18"/>
+      <c r="J14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="7" t="n">
+        <v>105</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10" t="n">
+      <c r="A15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="12" t="n">
+      <c r="F15" s="22" t="n">
         <v>1.5</v>
       </c>
-      <c r="G15" s="12" t="n">
+      <c r="G15" s="22" t="n">
         <v>2</v>
       </c>
+      <c r="I15" s="18"/>
+      <c r="J15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="7" t="n">
+        <v>145</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>0.81</v>
@@ -1599,11 +2233,24 @@
         <f aca="false">($D16)*(G$15)</f>
         <v>56.7</v>
       </c>
+      <c r="I16" s="18"/>
+      <c r="J16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="7" t="n">
+        <v>125</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="D17" s="4" t="n">
         <v>30</v>
@@ -1620,11 +2267,21 @@
         <f aca="false">($D17)*(G$15)</f>
         <v>60</v>
       </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="7" t="n">
+        <v>535</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>1.22</v>
@@ -1645,11 +2302,24 @@
         <f aca="false">($D18)*(G$15)</f>
         <v>61</v>
       </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" s="7" t="n">
+        <v>70</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>0.31</v>
@@ -1670,11 +2340,23 @@
         <f aca="false">($D19)*(G$15)</f>
         <v>62</v>
       </c>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" s="23" t="n">
+        <f aca="false">SUM(K2:K18)</f>
+        <v>3290</v>
+      </c>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>1.25</v>
@@ -1695,11 +2377,26 @@
         <f aca="false">($D20)*(G$15)</f>
         <v>62.5</v>
       </c>
+      <c r="I20" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K20" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M20" s="20" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>0.65</v>
@@ -1720,11 +2417,20 @@
         <f aca="false">($D21)*(G$15)</f>
         <v>65</v>
       </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K21" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="2" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>0.71</v>
@@ -1745,11 +2451,21 @@
         <f aca="false">($D22)*(G$15)</f>
         <v>71</v>
       </c>
+      <c r="I22" s="18"/>
+      <c r="J22" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="7" t="n">
+        <v>95</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D23" s="4" t="n">
         <v>36</v>
@@ -1766,11 +2482,21 @@
         <f aca="false">($D23)*(G$15)</f>
         <v>72</v>
       </c>
+      <c r="I23" s="18"/>
+      <c r="J23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="2" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>0.81</v>
@@ -1791,28 +2517,51 @@
         <f aca="false">($D24)*(G$15)</f>
         <v>81</v>
       </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" s="7" t="n">
+        <v>140</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10" t="n">
+      <c r="A25" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="12" t="n">
+      <c r="F25" s="22" t="n">
         <v>1.5</v>
       </c>
-      <c r="G25" s="12" t="n">
+      <c r="G25" s="22" t="n">
         <v>2</v>
       </c>
+      <c r="I25" s="18"/>
+      <c r="J25" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K25" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="L25" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D26" s="4" t="n">
         <v>100</v>
@@ -1829,11 +2578,22 @@
         <f aca="false">($D26)*(G$25)</f>
         <v>200</v>
       </c>
+      <c r="I26" s="18"/>
+      <c r="J26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="7" t="n">
+        <v>45</v>
+      </c>
+      <c r="L26" s="20"/>
+      <c r="M26" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="2" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="D27" s="4" t="n">
         <v>250</v>
@@ -1850,28 +2610,48 @@
         <f aca="false">($D27)*(G$25)</f>
         <v>500</v>
       </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K27" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10" t="n">
+      <c r="A28" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="F28" s="12" t="n">
+      <c r="F28" s="22" t="n">
         <v>1.5</v>
       </c>
-      <c r="G28" s="12" t="n">
+      <c r="G28" s="22" t="n">
         <v>2</v>
       </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K28" s="7" t="n">
+        <v>170</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="D29" s="4" t="n">
         <v>29</v>
@@ -1888,11 +2668,19 @@
         <f aca="false">($D29)*(G$28)</f>
         <v>58</v>
       </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K29" s="7" t="n">
+        <v>85</v>
+      </c>
+      <c r="L29" s="20"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="2" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="D30" s="4" t="n">
         <v>55</v>
@@ -1909,11 +2697,21 @@
         <f aca="false">($D30)*(G$28)</f>
         <v>110</v>
       </c>
+      <c r="I30" s="18"/>
+      <c r="J30" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K30" s="7" t="n">
+        <v>80</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="2" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="D31" s="4" t="n">
         <v>96</v>
@@ -1930,11 +2728,21 @@
         <f aca="false">($D31)*(G$28)</f>
         <v>192</v>
       </c>
+      <c r="I31" s="18"/>
+      <c r="J31" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K31" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="L31" s="20" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="D32" s="4" t="n">
         <v>112</v>
@@ -1951,11 +2759,19 @@
         <f aca="false">($D32)*(G$28)</f>
         <v>224</v>
       </c>
+      <c r="I32" s="18"/>
+      <c r="J32" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K32" s="7" t="n">
+        <v>55</v>
+      </c>
+      <c r="L32" s="20"/>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="2" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="D33" s="4" t="n">
         <v>138</v>
@@ -1972,20 +2788,732 @@
         <f aca="false">($D33)*(G$28)</f>
         <v>276</v>
       </c>
+      <c r="I33" s="18"/>
+      <c r="J33" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K33" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="L33" s="20"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I34" s="18"/>
+      <c r="J34" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K34" s="7" t="n">
+        <v>135</v>
+      </c>
+      <c r="L34" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M34" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I35" s="18"/>
+      <c r="J35" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K35" s="23" t="n">
+        <f aca="false">SUM(K20:K34)</f>
+        <v>1030</v>
+      </c>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I36" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K36" s="7" t="n">
+        <v>335</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="18"/>
+      <c r="J37" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K37" s="7" t="n">
+        <v>110</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="18"/>
+      <c r="J38" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K38" s="7" t="n">
+        <v>245</v>
+      </c>
+      <c r="L38" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I39" s="18"/>
+      <c r="J39" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K39" s="7" t="n">
+        <v>300</v>
+      </c>
+      <c r="L39" s="20"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I40" s="18"/>
+      <c r="J40" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="K40" s="7" t="n">
+        <v>60</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="M40" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I41" s="18"/>
+      <c r="J41" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K41" s="7" t="n">
+        <v>125</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I42" s="18"/>
+      <c r="J42" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K42" s="7" t="n">
+        <v>60</v>
+      </c>
+      <c r="L42" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I43" s="18"/>
+      <c r="J43" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K43" s="7" t="n">
+        <v>185</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I44" s="18"/>
+      <c r="J44" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K44" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I45" s="18"/>
+      <c r="J45" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K45" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M45" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I46" s="18"/>
+      <c r="J46" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K46" s="7" t="n">
+        <v>345</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="M46" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I47" s="18"/>
+      <c r="J47" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K47" s="7" t="n">
+        <v>215</v>
+      </c>
+      <c r="L47" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I48" s="18"/>
+      <c r="J48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K48" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L48" s="20"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I49" s="18"/>
+      <c r="J49" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K49" s="7" t="n">
+        <v>325</v>
+      </c>
+      <c r="L49" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M49" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I50" s="18"/>
+      <c r="J50" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K50" s="23" t="n">
+        <f aca="false">SUM(K36:K49)</f>
+        <v>2470</v>
+      </c>
+      <c r="L50" s="24"/>
+      <c r="M50" s="24"/>
+      <c r="N50" s="25"/>
+      <c r="O50" s="25"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I51" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="K51" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="L51" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I52" s="18"/>
+      <c r="J52" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K52" s="7" t="n">
+        <v>90</v>
+      </c>
+      <c r="L52" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M52" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I53" s="18"/>
+      <c r="J53" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K53" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M53" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I54" s="18"/>
+      <c r="J54" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K54" s="7" t="n">
+        <v>80</v>
+      </c>
+      <c r="L54" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I55" s="18"/>
+      <c r="J55" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K55" s="7" t="n">
+        <v>1060</v>
+      </c>
+      <c r="L55" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I56" s="18"/>
+      <c r="J56" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="K56" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="L56" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M56" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I57" s="18"/>
+      <c r="J57" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K57" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I58" s="18"/>
+      <c r="J58" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K58" s="23" t="n">
+        <f aca="false">SUM(K51:K57)</f>
+        <v>1335</v>
+      </c>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="25"/>
+      <c r="O58" s="25"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I59" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K59" s="7" t="n">
+        <v>110</v>
+      </c>
+      <c r="L59" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M59" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I60" s="18"/>
+      <c r="J60" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="K60" s="7" t="n">
+        <v>140</v>
+      </c>
+      <c r="L60" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I61" s="18"/>
+      <c r="J61" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K61" s="7" t="n">
+        <v>65</v>
+      </c>
+      <c r="L61" s="20"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I62" s="18"/>
+      <c r="J62" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K62" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L62" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M62" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I63" s="18"/>
+      <c r="J63" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K63" s="7" t="n">
+        <v>65</v>
+      </c>
+      <c r="L63" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I64" s="18"/>
+      <c r="J64" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K64" s="7" t="n">
+        <v>95</v>
+      </c>
+      <c r="L64" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M64" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I65" s="18"/>
+      <c r="J65" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="K65" s="7" t="n">
+        <v>135</v>
+      </c>
+      <c r="L65" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="M65" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I66" s="18"/>
+      <c r="J66" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="K66" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="L66" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="M66" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I67" s="18"/>
+      <c r="J67" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K67" s="7" t="n">
+        <v>65</v>
+      </c>
+      <c r="L67" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="M67" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I68" s="18"/>
+      <c r="J68" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="K68" s="7" t="n">
+        <v>1260</v>
+      </c>
+      <c r="L68" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M68" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I69" s="18"/>
+      <c r="J69" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="K69" s="7" t="n">
+        <v>45</v>
+      </c>
+      <c r="L69" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M69" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I70" s="18"/>
+      <c r="J70" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K70" s="7" t="n">
+        <v>70</v>
+      </c>
+      <c r="L70" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I71" s="18"/>
+      <c r="J71" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K71" s="7" t="n">
+        <v>190</v>
+      </c>
+      <c r="L71" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I72" s="18"/>
+      <c r="J72" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K72" s="7" t="n">
+        <v>130</v>
+      </c>
+      <c r="L72" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I73" s="18"/>
+      <c r="J73" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K73" s="7" t="n">
+        <v>95</v>
+      </c>
+      <c r="L73" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="M73" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I74" s="18"/>
+      <c r="J74" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K74" s="7" t="n">
+        <v>150</v>
+      </c>
+      <c r="L74" s="20"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I75" s="18"/>
+      <c r="J75" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K75" s="7" t="n">
+        <v>145</v>
+      </c>
+      <c r="L75" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I76" s="18"/>
+      <c r="J76" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K76" s="23" t="n">
+        <f aca="false">SUM(K59:K75)</f>
+        <v>3010</v>
+      </c>
+      <c r="L76" s="24"/>
+      <c r="M76" s="24"/>
+      <c r="N76" s="25"/>
+      <c r="O76" s="25"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I77" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K77" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="L77" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="M77" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I78" s="18"/>
+      <c r="J78" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K78" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L78" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I79" s="18"/>
+      <c r="J79" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K79" s="7" t="n">
+        <v>230</v>
+      </c>
+      <c r="L79" s="20"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I80" s="18"/>
+      <c r="J80" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K80" s="7" t="n">
+        <v>615</v>
+      </c>
+      <c r="L80" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="M80" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I81" s="18"/>
+      <c r="J81" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="K81" s="7" t="n">
+        <v>135</v>
+      </c>
+      <c r="L81" s="20"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I82" s="18"/>
+      <c r="J82" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="K82" s="7" t="n">
+        <v>1075</v>
+      </c>
+      <c r="L82" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I83" s="18"/>
+      <c r="J83" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K83" s="23" t="n">
+        <f aca="false">SUM(K77:K82)</f>
+        <v>2175</v>
+      </c>
+      <c r="L83" s="24"/>
+      <c r="M83" s="24"/>
+      <c r="N83" s="25"/>
+      <c r="O83" s="25"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I84" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="J84" s="18"/>
+      <c r="K84" s="26" t="n">
+        <f aca="false">SUM(K19,K35,K50,K58,K76,K83)</f>
+        <v>13310</v>
+      </c>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
+      <c r="N84" s="27"/>
+      <c r="O84" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="34">
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="I2:I19"/>
+    <mergeCell ref="M3:M6"/>
+    <mergeCell ref="L4:L6"/>
     <mergeCell ref="A7:A14"/>
     <mergeCell ref="B7:D7"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
     <mergeCell ref="A15:A24"/>
     <mergeCell ref="B15:D15"/>
+    <mergeCell ref="I20:I35"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M20:M21"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B25:D25"/>
+    <mergeCell ref="L25:L26"/>
     <mergeCell ref="A28:A33"/>
     <mergeCell ref="B28:D28"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="I36:I50"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="I51:I58"/>
+    <mergeCell ref="L56:L57"/>
+    <mergeCell ref="I59:I76"/>
+    <mergeCell ref="L60:L61"/>
+    <mergeCell ref="L73:L74"/>
+    <mergeCell ref="I77:I83"/>
+    <mergeCell ref="L78:L79"/>
+    <mergeCell ref="L80:L81"/>
+    <mergeCell ref="I84:J84"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>